<commit_message>
adapted for changes to introduce 'register file' layer
</commit_message>
<xml_diff>
--- a/spec/files/test.xlsx
+++ b/spec/files/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ishitani\workspace\rggen-spreadsheet-loader\spec\support\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ishitani\workspace\rggen-spreadsheet-loader\spec\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58E760C-B993-44EA-9B55-091426577165}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EECAD3-756C-4EE6-A56A-C89761B6D8D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{545F8173-9CE8-4C56-A444-A44B312815E6}"/>
   </bookViews>
@@ -595,7 +595,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F615CE7-CBE6-494D-A46A-A725DC3F8EF8}">
-  <dimension ref="B1:E7"/>
+  <dimension ref="B1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -651,25 +651,25 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B6" t="s">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>25</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="D7" t="s">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>